<commit_message>
separate CO2 emission from CH4 characterization factor
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/oilcane/results/life_cycle.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/oilcane/results/life_cycle.xlsx
@@ -450,7 +450,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -501,7 +501,7 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>5915485.974851853</v>
+        <v>5915485.974855063</v>
       </c>
     </row>
     <row r="3">
@@ -515,13 +515,13 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>677618.0597347515</v>
+        <v>677618.0597347516</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>621522.7695020641</v>
+        <v>621522.7695024513</v>
       </c>
     </row>
     <row r="4">
@@ -535,13 +535,13 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>78965.33896108529</v>
+        <v>78965.33896108548</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>82382.39289191431</v>
+        <v>82382.3928919235</v>
       </c>
     </row>
     <row r="5">
@@ -635,13 +635,13 @@
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>7800270.893413329</v>
+        <v>7800270.893414853</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>6725685.691953307</v>
+        <v>6725685.691957544</v>
       </c>
     </row>
     <row r="10">
@@ -661,7 +661,7 @@
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>47631282.15033584</v>
+        <v>47631282.15033583</v>
       </c>
     </row>
     <row r="11">
@@ -698,7 +698,7 @@
         <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>13728715.15243592</v>
+        <v>13728715.15243591</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
@@ -755,13 +755,13 @@
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>9730401.230924385</v>
+        <v>9730401.230924917</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>41386304.23720036</v>
+        <v>39805621.18948559</v>
       </c>
     </row>
     <row r="16">
@@ -825,93 +825,133 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="inlineStr">
+      <c r="A19" s="1" t="n"/>
+      <c r="B19" s="1" t="inlineStr">
+        <is>
+          <t>Electricity [kWhr/yr]</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
         <is>
           <t>Outputs</t>
         </is>
       </c>
-      <c r="B19" s="1" t="inlineStr">
+      <c r="B20" s="1" t="inlineStr">
         <is>
           <t>Biodiesel</t>
         </is>
       </c>
-      <c r="C19" t="n">
-        <v>0</v>
-      </c>
-      <c r="D19" t="n">
-        <v>0</v>
-      </c>
-      <c r="E19" t="n">
+      <c r="C20" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" t="n">
         <v>14070407.71607705</v>
       </c>
-      <c r="F19" t="n">
+      <c r="F20" t="n">
         <v>17009797.33833415</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="n"/>
-      <c r="B20" s="1" t="inlineStr">
-        <is>
-          <t>Crude glycerol</t>
-        </is>
-      </c>
-      <c r="C20" t="n">
-        <v>0</v>
-      </c>
-      <c r="D20" t="n">
-        <v>0</v>
-      </c>
-      <c r="E20" t="n">
-        <v>3657354.837900585</v>
-      </c>
-      <c r="F20" t="n">
-        <v>4421357.459088729</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n"/>
       <c r="B21" s="1" t="inlineStr">
         <is>
-          <t>Ethanol</t>
+          <t>Crude glycerol</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>111916476.7675769</v>
+        <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>165569691.6327289</v>
+        <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>84288375.21843551</v>
+        <v>3657354.837900585</v>
       </c>
       <c r="F21" t="n">
-        <v>145786967.9368376</v>
+        <v>4421357.459088729</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n"/>
       <c r="B22" s="1" t="inlineStr">
         <is>
+          <t>Ethanol</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>111916476.7675769</v>
+      </c>
+      <c r="D22" t="n">
+        <v>165569691.6327289</v>
+      </c>
+      <c r="E22" t="n">
+        <v>84288375.21843551</v>
+      </c>
+      <c r="F22" t="n">
+        <v>145786967.9368376</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n"/>
+      <c r="B23" s="1" t="inlineStr">
+        <is>
           <t>Electricity [kWhr/yr]</t>
         </is>
       </c>
-      <c r="C22" t="n">
-        <v>295214880.9294902</v>
-      </c>
-      <c r="D22" t="n">
-        <v>2.564775058999658e-08</v>
-      </c>
-      <c r="E22" t="n">
-        <v>394423741.1527265</v>
-      </c>
-      <c r="F22" t="n">
-        <v>6.380389550031396e-08</v>
+      <c r="C23" t="n">
+        <v>295214880.9294904</v>
+      </c>
+      <c r="D23" t="n">
+        <v>4.365574568510056e-08</v>
+      </c>
+      <c r="E23" t="n">
+        <v>394423741.1516488</v>
+      </c>
+      <c r="F23" t="n">
+        <v>9.894165486912243e-08</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>Direct non-biogenic emissions</t>
+        </is>
+      </c>
+      <c r="B24" s="1" t="inlineStr"/>
+      <c r="C24" t="n">
+        <v>31477099.02498162</v>
+      </c>
+      <c r="D24" t="n">
+        <v>26693542.8215118</v>
+      </c>
+      <c r="E24" t="n">
+        <v>37662172.10459796</v>
+      </c>
+      <c r="F24" t="n">
+        <v>109199305.2024856</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A2:A18"/>
-    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="A2:A19"/>
+    <mergeCell ref="A20:A23"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -923,7 +963,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -982,7 +1022,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>0.06329892343166782</v>
+        <v>0.06329892343170215</v>
       </c>
     </row>
     <row r="3">
@@ -1005,7 +1045,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>0.007076954901897844</v>
+        <v>0.007076954901902252</v>
       </c>
     </row>
     <row r="4">
@@ -1022,13 +1062,13 @@
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0002503716700416491</v>
+        <v>0.0002503716700416496</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0002966505930821476</v>
+        <v>0.0002966505930821807</v>
       </c>
     </row>
     <row r="5">
@@ -1137,13 +1177,13 @@
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>0.04734726610030584</v>
+        <v>0.04734726610031509</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>0.04636432334158672</v>
+        <v>0.04636432334161593</v>
       </c>
     </row>
     <row r="10">
@@ -1166,7 +1206,7 @@
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>0.05273234671013193</v>
+        <v>0.05273234671013192</v>
       </c>
     </row>
     <row r="11">
@@ -1200,16 +1240,16 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>3.073313681318202</v>
+        <v>0.33</v>
       </c>
       <c r="D12" t="n">
-        <v>0.3150881646555273</v>
+        <v>0.03383289345581067</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>0.5005749368825591</v>
+        <v>0.0537497132737819</v>
       </c>
       <c r="G12" t="n">
         <v>0</v>
@@ -1269,19 +1309,19 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>3.073313681318202</v>
+        <v>0.33</v>
       </c>
       <c r="D15" t="n">
         <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>0.1806162404049801</v>
+        <v>0.01939384179882403</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>0.8724586074558595</v>
+        <v>0.09010308108075461</v>
       </c>
     </row>
     <row r="16">
@@ -1301,10 +1341,10 @@
         <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>0.6676507877475601</v>
+        <v>0.66765078774756</v>
       </c>
       <c r="G16" t="n">
-        <v>0.3860098121865853</v>
+        <v>0.3860098121865852</v>
       </c>
     </row>
     <row r="17">
@@ -1354,147 +1394,197 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="inlineStr">
-        <is>
-          <t>Total inputs</t>
-        </is>
-      </c>
-      <c r="B19" s="1" t="inlineStr"/>
-      <c r="C19" t="inlineStr"/>
+      <c r="A19" s="1" t="n"/>
+      <c r="B19" s="1" t="inlineStr">
+        <is>
+          <t>Electricity</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>0</v>
+      </c>
       <c r="D19" t="n">
-        <v>0.8439169448368461</v>
+        <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>0.6994142198784308</v>
+        <v>0</v>
       </c>
       <c r="F19" t="n">
-        <v>1.233474331349373</v>
+        <v>0</v>
       </c>
       <c r="G19" t="n">
-        <v>1.480129877906659</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
+          <t>Total inputs</t>
+        </is>
+      </c>
+      <c r="B20" s="1" t="inlineStr"/>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="n">
+        <v>0.5626616736371295</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.5381918212722838</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.7866491077405956</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.6977743515316223</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
           <t>Outputs displaced</t>
         </is>
       </c>
-      <c r="B20" s="1" t="inlineStr">
+      <c r="B21" s="1" t="inlineStr">
         <is>
           <t>Biodiesel</t>
         </is>
       </c>
-      <c r="C20" t="n">
+      <c r="C21" t="n">
         <v>1.13</v>
       </c>
-      <c r="D20" t="n">
-        <v>0</v>
-      </c>
-      <c r="E20" t="n">
-        <v>0</v>
-      </c>
-      <c r="F20" t="n">
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" t="n">
         <v>0.1886329007762095</v>
       </c>
-      <c r="G20" t="n">
+      <c r="G21" t="n">
         <v>0.1318435472273842</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="n"/>
-      <c r="B21" s="1" t="inlineStr">
-        <is>
-          <t>Crude glycerol</t>
-        </is>
-      </c>
-      <c r="C21" t="n">
-        <v>0.288</v>
-      </c>
-      <c r="D21" t="n">
-        <v>0</v>
-      </c>
-      <c r="E21" t="n">
-        <v>0</v>
-      </c>
-      <c r="F21" t="n">
-        <v>0.01249660099136645</v>
-      </c>
-      <c r="G21" t="n">
-        <v>0.008734326299791317</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n"/>
       <c r="B22" s="1" t="inlineStr">
         <is>
+          <t>Crude glycerol</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>0.288</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.01249660099136645</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.008734326299791317</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n"/>
+      <c r="B23" s="1" t="inlineStr">
+        <is>
           <t>Electricity</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="C23" t="inlineStr">
         <is>
           <t>0.36 kg*CO2e/kWhr</t>
         </is>
       </c>
-      <c r="D22" t="n">
-        <v>0.9496131419087513</v>
-      </c>
-      <c r="E22" t="n">
-        <v>5.576618595678776e-17</v>
-      </c>
-      <c r="F22" t="n">
-        <v>1.684604151485946</v>
-      </c>
-      <c r="G22" t="n">
-        <v>1.575545654400643e-16</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="inlineStr">
-        <is>
-          <t>Total outputs displaced</t>
-        </is>
-      </c>
-      <c r="B23" s="1" t="inlineStr"/>
-      <c r="C23" t="inlineStr"/>
       <c r="D23" t="n">
-        <v>0.9496131419087513</v>
+        <v>0.949613141908752</v>
       </c>
       <c r="E23" t="n">
-        <v>5.576618595678776e-17</v>
+        <v>9.492116758602173e-17</v>
       </c>
       <c r="F23" t="n">
-        <v>1.885733653253522</v>
+        <v>1.684604151481342</v>
       </c>
       <c r="G23" t="n">
-        <v>0.1405778735271757</v>
+        <v>2.443222206824143e-16</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>Total</t>
+          <t>Total outputs displaced</t>
         </is>
       </c>
       <c r="B24" s="1" t="inlineStr"/>
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="n">
-        <v>-0.1056961970719053</v>
+        <v>0.949613141908752</v>
       </c>
       <c r="E24" t="n">
-        <v>0.6994142198784307</v>
+        <v>9.492116758602173e-17</v>
       </c>
       <c r="F24" t="n">
-        <v>-0.6522593219041488</v>
+        <v>1.885733653248918</v>
       </c>
       <c r="G24" t="n">
-        <v>1.339552004379484</v>
+        <v>0.1405778735271758</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>Process impacts</t>
+        </is>
+      </c>
+      <c r="B25" s="1" t="inlineStr">
+        <is>
+          <t>Direct non-biogenic emissions</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>1</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.2812552711997166</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.1612223986061659</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.4468252236087771</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0.7490333789629011</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B26" s="1" t="inlineStr"/>
+      <c r="C26" t="inlineStr"/>
+      <c r="D26" t="n">
+        <v>-0.1056961970719059</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.6994142198784497</v>
+      </c>
+      <c r="F26" t="n">
+        <v>-0.6522593218995458</v>
+      </c>
+      <c r="G26" t="n">
+        <v>1.306229856967348</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A2:A18"/>
-    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="A2:A19"/>
+    <mergeCell ref="A21:A23"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1549,7 +1639,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1235404575672317</v>
+        <v>0.1235404575673441</v>
       </c>
       <c r="E2" t="n">
         <v>0.1377966870439366</v>
@@ -1568,10 +1658,10 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0106002423898781</v>
+        <v>0.01060024238988774</v>
       </c>
       <c r="E3" t="n">
-        <v>0.01182348122121565</v>
+        <v>0.01182348122121566</v>
       </c>
     </row>
     <row r="4">
@@ -1581,16 +1671,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.2604907241031162</v>
+        <v>0.2604907241031163</v>
       </c>
       <c r="C4" t="n">
-        <v>2.816793302774396e-17</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0.3329849492228651</v>
+        <v>0.3329849492222581</v>
       </c>
       <c r="E4" t="n">
-        <v>4.080574642082992e-17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -1606,10 +1696,10 @@
         <v>1</v>
       </c>
       <c r="D5" t="n">
-        <v>0.5328743508200251</v>
+        <v>0.53287435082051</v>
       </c>
       <c r="E5" t="n">
-        <v>0.8503798317348478</v>
+        <v>0.8503798317348477</v>
       </c>
     </row>
   </sheetData>
@@ -1666,7 +1756,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1641377906350205</v>
+        <v>0.1641377906351399</v>
       </c>
       <c r="E2" t="n">
         <v>0.1680530358447928</v>
@@ -1685,10 +1775,10 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0.00615836792245201</v>
+        <v>0.006158367922456488</v>
       </c>
       <c r="E3" t="n">
-        <v>0.006305208958143325</v>
+        <v>0.006305208958143326</v>
       </c>
     </row>
     <row r="4">
@@ -1698,16 +1788,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.2101761441374755</v>
+        <v>0.2101761441374756</v>
       </c>
       <c r="C4" t="n">
-        <v>2.127940672645292e-17</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0.266072278559137</v>
+        <v>0.2660722785586033</v>
       </c>
       <c r="E4" t="n">
-        <v>2.992985131427244e-17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -1723,7 +1813,7 @@
         <v>1</v>
       </c>
       <c r="D5" t="n">
-        <v>0.5636315628833904</v>
+        <v>0.5636315628838003</v>
       </c>
       <c r="E5" t="n">
         <v>0.8256417551970638</v>
@@ -1783,10 +1873,10 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1529281120668742</v>
+        <v>0.1529281120668743</v>
       </c>
       <c r="E2" t="n">
-        <v>0.08907566099121637</v>
+        <v>0.09112720677979762</v>
       </c>
     </row>
     <row r="3">
@@ -1802,10 +1892,10 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0.01013122095349617</v>
+        <v>0.01013122095349618</v>
       </c>
       <c r="E3" t="n">
-        <v>0.005901053975171445</v>
+        <v>0.006036964080089546</v>
       </c>
     </row>
     <row r="4">
@@ -1815,16 +1905,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1.125244785898142</v>
+        <v>1.125244785898143</v>
       </c>
       <c r="C4" t="n">
-        <v>1.085721907141328e-16</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>1.365739122956093</v>
+        <v>1.365739122952361</v>
       </c>
       <c r="E4" t="n">
-        <v>-5.071301927276078e-17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -1834,16 +1924,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.1252447858981424</v>
+        <v>-0.1252447858981433</v>
       </c>
       <c r="C5" t="n">
-        <v>0.9999999999999999</v>
+        <v>1</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.528798455976463</v>
+        <v>-0.5287984559727319</v>
       </c>
       <c r="E5" t="n">
-        <v>0.9050232850336122</v>
+        <v>0.9028358291401126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
use new biosteam features for process impacts
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/oilcane/results/life_cycle.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/oilcane/results/life_cycle.xlsx
@@ -919,13 +919,13 @@
         <v>295214880.9294904</v>
       </c>
       <c r="D23" t="n">
-        <v>4.365574568510056e-08</v>
+        <v>8.671463547216263e-08</v>
       </c>
       <c r="E23" t="n">
-        <v>394423741.1516488</v>
+        <v>394423741.1516486</v>
       </c>
       <c r="F23" t="n">
-        <v>9.894165486912243e-08</v>
+        <v>8.731682044071931e-08</v>
       </c>
     </row>
     <row r="24">
@@ -1500,16 +1500,16 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>0.949613141908752</v>
+        <v>0.9496131419087521</v>
       </c>
       <c r="E23" t="n">
-        <v>9.492116758602173e-17</v>
+        <v>1.885445848339533e-16</v>
       </c>
       <c r="F23" t="n">
         <v>1.684604151481342</v>
       </c>
       <c r="G23" t="n">
-        <v>2.443222206824143e-16</v>
+        <v>2.156163599772362e-16</v>
       </c>
     </row>
     <row r="24">
@@ -1521,16 +1521,16 @@
       <c r="B24" s="1" t="inlineStr"/>
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="n">
-        <v>0.949613141908752</v>
+        <v>0.9496131419087521</v>
       </c>
       <c r="E24" t="n">
-        <v>9.492116758602173e-17</v>
+        <v>1.885445848339533e-16</v>
       </c>
       <c r="F24" t="n">
         <v>1.885733653248918</v>
       </c>
       <c r="G24" t="n">
-        <v>0.1405778735271758</v>
+        <v>0.1405778735271757</v>
       </c>
     </row>
     <row r="25">
@@ -1569,13 +1569,13 @@
       <c r="B26" s="1" t="inlineStr"/>
       <c r="C26" t="inlineStr"/>
       <c r="D26" t="n">
-        <v>-0.1056961970719059</v>
+        <v>-0.105696197071906</v>
       </c>
       <c r="E26" t="n">
-        <v>0.6994142198784497</v>
+        <v>0.6994142198784495</v>
       </c>
       <c r="F26" t="n">
-        <v>-0.6522593218995458</v>
+        <v>-0.6522593218995449</v>
       </c>
       <c r="G26" t="n">
         <v>1.306229856967348</v>
@@ -1696,7 +1696,7 @@
         <v>1</v>
       </c>
       <c r="D5" t="n">
-        <v>0.53287435082051</v>
+        <v>0.5328743508205099</v>
       </c>
       <c r="E5" t="n">
         <v>0.8503798317348477</v>
@@ -1775,7 +1775,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0.006158367922456488</v>
+        <v>0.006158367922456487</v>
       </c>
       <c r="E3" t="n">
         <v>0.006305208958143326</v>
@@ -1813,7 +1813,7 @@
         <v>1</v>
       </c>
       <c r="D5" t="n">
-        <v>0.5636315628838003</v>
+        <v>0.5636315628838002</v>
       </c>
       <c r="E5" t="n">
         <v>0.8256417551970638</v>
@@ -1873,10 +1873,10 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1529281120668743</v>
+        <v>0.1529281120668742</v>
       </c>
       <c r="E2" t="n">
-        <v>0.09112720677979762</v>
+        <v>0.09112720677979763</v>
       </c>
     </row>
     <row r="3">
@@ -1892,10 +1892,10 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0.01013122095349618</v>
+        <v>0.01013122095349617</v>
       </c>
       <c r="E3" t="n">
-        <v>0.006036964080089546</v>
+        <v>0.006036964080089547</v>
       </c>
     </row>
     <row r="4">
@@ -1905,7 +1905,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1.125244785898143</v>
+        <v>1.125244785898144</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
@@ -1924,16 +1924,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.1252447858981433</v>
+        <v>-0.1252447858981437</v>
       </c>
       <c r="C5" t="n">
         <v>1</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.5287984559727319</v>
+        <v>-0.5287984559727309</v>
       </c>
       <c r="E5" t="n">
-        <v>0.9028358291401126</v>
+        <v>0.9028358291401128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
use set_CF for setting power utility for better practice
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/oilcane/results/life_cycle.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/oilcane/results/life_cycle.xlsx
@@ -450,7 +450,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -501,7 +501,7 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>5915485.974855063</v>
+        <v>5915485.974851853</v>
       </c>
     </row>
     <row r="3">
@@ -515,13 +515,13 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>677618.0597347516</v>
+        <v>677618.0597347515</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>621522.7695024513</v>
+        <v>621522.7695020641</v>
       </c>
     </row>
     <row r="4">
@@ -535,13 +535,13 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>78965.33896108548</v>
+        <v>78965.33896108529</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>82382.3928919235</v>
+        <v>82382.39289191431</v>
       </c>
     </row>
     <row r="5">
@@ -635,13 +635,13 @@
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>7800270.893414853</v>
+        <v>7800270.893413329</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>6725685.691957544</v>
+        <v>6725685.691953307</v>
       </c>
     </row>
     <row r="10">
@@ -661,7 +661,7 @@
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>47631282.15033583</v>
+        <v>47631282.15033584</v>
       </c>
     </row>
     <row r="11">
@@ -698,7 +698,7 @@
         <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>13728715.15243591</v>
+        <v>13728715.15243592</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
@@ -755,13 +755,13 @@
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>9730401.230924917</v>
+        <v>9730401.230924385</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>39805621.18948559</v>
+        <v>41386304.23720033</v>
       </c>
     </row>
     <row r="16">
@@ -825,10 +825,14 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="n"/>
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>Outputs</t>
+        </is>
+      </c>
       <c r="B19" s="1" t="inlineStr">
         <is>
-          <t>Electricity [kWhr/yr]</t>
+          <t>Biodiesel</t>
         </is>
       </c>
       <c r="C19" t="n">
@@ -838,21 +842,17 @@
         <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>0</v>
+        <v>14070407.71607705</v>
       </c>
       <c r="F19" t="n">
-        <v>0</v>
+        <v>17009797.33833415</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="inlineStr">
-        <is>
-          <t>Outputs</t>
-        </is>
-      </c>
+      <c r="A20" s="1" t="n"/>
       <c r="B20" s="1" t="inlineStr">
         <is>
-          <t>Biodiesel</t>
+          <t>Crude glycerol</t>
         </is>
       </c>
       <c r="C20" t="n">
@@ -862,96 +862,76 @@
         <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>14070407.71607705</v>
+        <v>3657354.837900585</v>
       </c>
       <c r="F20" t="n">
-        <v>17009797.33833415</v>
+        <v>4421357.459088729</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n"/>
       <c r="B21" s="1" t="inlineStr">
         <is>
-          <t>Crude glycerol</t>
+          <t>Ethanol</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0</v>
+        <v>111916476.7675769</v>
       </c>
       <c r="D21" t="n">
-        <v>0</v>
+        <v>165569691.6327289</v>
       </c>
       <c r="E21" t="n">
-        <v>3657354.837900585</v>
+        <v>84288375.21843551</v>
       </c>
       <c r="F21" t="n">
-        <v>4421357.459088729</v>
+        <v>145786967.9368376</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n"/>
       <c r="B22" s="1" t="inlineStr">
         <is>
-          <t>Ethanol</t>
+          <t>Electricity [kWhr/yr]</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>111916476.7675769</v>
+        <v>295214880.9294902</v>
       </c>
       <c r="D22" t="n">
-        <v>165569691.6327289</v>
+        <v>-0</v>
       </c>
       <c r="E22" t="n">
-        <v>84288375.21843551</v>
+        <v>394423741.1527265</v>
       </c>
       <c r="F22" t="n">
-        <v>145786967.9368376</v>
+        <v>3.492459654808044e-08</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="1" t="n"/>
-      <c r="B23" s="1" t="inlineStr">
-        <is>
-          <t>Electricity [kWhr/yr]</t>
-        </is>
-      </c>
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>Direct non-biogenic emissions</t>
+        </is>
+      </c>
+      <c r="B23" s="1" t="inlineStr"/>
       <c r="C23" t="n">
-        <v>295214880.9294904</v>
+        <v>31477099.02498162</v>
       </c>
       <c r="D23" t="n">
-        <v>8.671463547216263e-08</v>
+        <v>26693542.82151034</v>
       </c>
       <c r="E23" t="n">
-        <v>394423741.1516486</v>
+        <v>37662172.10459796</v>
       </c>
       <c r="F23" t="n">
-        <v>8.731682044071931e-08</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="inlineStr">
-        <is>
-          <t>Direct non-biogenic emissions</t>
-        </is>
-      </c>
-      <c r="B24" s="1" t="inlineStr"/>
-      <c r="C24" t="n">
-        <v>31477099.02498162</v>
-      </c>
-      <c r="D24" t="n">
-        <v>26693542.8215118</v>
-      </c>
-      <c r="E24" t="n">
-        <v>37662172.10459796</v>
-      </c>
-      <c r="F24" t="n">
-        <v>109199305.2024856</v>
+        <v>113535614.6331092</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A2:A19"/>
-    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A2:A18"/>
+    <mergeCell ref="A19:A22"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -963,7 +943,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1022,7 +1002,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>0.06329892343170215</v>
+        <v>0.06329892343166782</v>
       </c>
     </row>
     <row r="3">
@@ -1045,7 +1025,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>0.007076954901902252</v>
+        <v>0.007076954901897844</v>
       </c>
     </row>
     <row r="4">
@@ -1062,13 +1042,13 @@
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0002503716700416496</v>
+        <v>0.0002503716700416491</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0002966505930821807</v>
+        <v>0.0002966505930821476</v>
       </c>
     </row>
     <row r="5">
@@ -1177,13 +1157,13 @@
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>0.04734726610031509</v>
+        <v>0.04734726610030584</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>0.04636432334161593</v>
+        <v>0.04636432334158672</v>
       </c>
     </row>
     <row r="10">
@@ -1206,7 +1186,7 @@
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>0.05273234671013192</v>
+        <v>0.05273234671013193</v>
       </c>
     </row>
     <row r="11">
@@ -1315,13 +1295,13 @@
         <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>0.01939384179882403</v>
+        <v>0.01939384179882297</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>0.09010308108075461</v>
+        <v>0.09368107857345134</v>
       </c>
     </row>
     <row r="16">
@@ -1341,10 +1321,10 @@
         <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>0.66765078774756</v>
+        <v>0.6676507877475601</v>
       </c>
       <c r="G16" t="n">
-        <v>0.3860098121865852</v>
+        <v>0.3860098121865853</v>
       </c>
     </row>
     <row r="17">
@@ -1394,62 +1374,62 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="n"/>
-      <c r="B19" s="1" t="inlineStr">
-        <is>
-          <t>Electricity</t>
-        </is>
-      </c>
-      <c r="C19" t="n">
-        <v>0</v>
-      </c>
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>Total inputs</t>
+        </is>
+      </c>
+      <c r="B19" s="1" t="inlineStr"/>
+      <c r="C19" t="inlineStr"/>
       <c r="D19" t="n">
-        <v>0</v>
+        <v>0.5626616736371295</v>
       </c>
       <c r="E19" t="n">
-        <v>0</v>
+        <v>0.5381918212722736</v>
       </c>
       <c r="F19" t="n">
-        <v>0</v>
+        <v>0.7866491077405957</v>
       </c>
       <c r="G19" t="n">
-        <v>0</v>
+        <v>0.7013523490242511</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>Total inputs</t>
-        </is>
-      </c>
-      <c r="B20" s="1" t="inlineStr"/>
-      <c r="C20" t="inlineStr"/>
+          <t>Outputs displaced</t>
+        </is>
+      </c>
+      <c r="B20" s="1" t="inlineStr">
+        <is>
+          <t>Biodiesel</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>3.511317056376417</v>
+      </c>
       <c r="D20" t="n">
-        <v>0.5626616736371295</v>
+        <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>0.5381918212722838</v>
+        <v>0</v>
       </c>
       <c r="F20" t="n">
-        <v>0.7866491077405956</v>
+        <v>0.5861503733533318</v>
       </c>
       <c r="G20" t="n">
-        <v>0.6977743515316223</v>
+        <v>0.4096853948253839</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="1" t="inlineStr">
-        <is>
-          <t>Outputs displaced</t>
-        </is>
-      </c>
+      <c r="A21" s="1" t="n"/>
       <c r="B21" s="1" t="inlineStr">
         <is>
-          <t>Biodiesel</t>
+          <t>Crude glycerol</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>1.13</v>
+        <v>0.288</v>
       </c>
       <c r="D21" t="n">
         <v>0</v>
@@ -1458,133 +1438,110 @@
         <v>0</v>
       </c>
       <c r="F21" t="n">
-        <v>0.1886329007762095</v>
+        <v>0.01249660099136645</v>
       </c>
       <c r="G21" t="n">
-        <v>0.1318435472273842</v>
+        <v>0.008734326299791317</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n"/>
       <c r="B22" s="1" t="inlineStr">
         <is>
-          <t>Crude glycerol</t>
-        </is>
-      </c>
-      <c r="C22" t="n">
-        <v>0.288</v>
+          <t>Electricity</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>0.36 kg*CO2e/kWhr</t>
+        </is>
       </c>
       <c r="D22" t="n">
-        <v>0</v>
+        <v>0.9496131419087513</v>
       </c>
       <c r="E22" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="F22" t="n">
-        <v>0.01249660099136645</v>
+        <v>1.684604151485945</v>
       </c>
       <c r="G22" t="n">
-        <v>0.008734326299791317</v>
+        <v>8.624128024087976e-17</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="1" t="n"/>
-      <c r="B23" s="1" t="inlineStr">
-        <is>
-          <t>Electricity</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>0.36 kg*CO2e/kWhr</t>
-        </is>
-      </c>
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>Total outputs displaced</t>
+        </is>
+      </c>
+      <c r="B23" s="1" t="inlineStr"/>
+      <c r="C23" t="inlineStr"/>
       <c r="D23" t="n">
-        <v>0.9496131419087521</v>
+        <v>0.9496131419087513</v>
       </c>
       <c r="E23" t="n">
-        <v>1.885445848339533e-16</v>
+        <v>0</v>
       </c>
       <c r="F23" t="n">
-        <v>1.684604151481342</v>
+        <v>2.283251125830643</v>
       </c>
       <c r="G23" t="n">
-        <v>2.156163599772362e-16</v>
+        <v>0.4184197211251753</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>Total outputs displaced</t>
-        </is>
-      </c>
-      <c r="B24" s="1" t="inlineStr"/>
-      <c r="C24" t="inlineStr"/>
+          <t>Process impacts</t>
+        </is>
+      </c>
+      <c r="B24" s="1" t="inlineStr">
+        <is>
+          <t>Direct non-biogenic emissions</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>1</v>
+      </c>
       <c r="D24" t="n">
-        <v>0.9496131419087521</v>
+        <v>0.2812552711997166</v>
       </c>
       <c r="E24" t="n">
-        <v>1.885445848339533e-16</v>
+        <v>0.1612223986061571</v>
       </c>
       <c r="F24" t="n">
-        <v>1.885733653248918</v>
+        <v>0.4468252236087771</v>
       </c>
       <c r="G24" t="n">
-        <v>0.1405778735271757</v>
+        <v>0.7787775288824078</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>Process impacts</t>
-        </is>
-      </c>
-      <c r="B25" s="1" t="inlineStr">
-        <is>
-          <t>Direct non-biogenic emissions</t>
-        </is>
-      </c>
-      <c r="C25" t="n">
-        <v>1</v>
-      </c>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B25" s="1" t="inlineStr"/>
+      <c r="C25" t="inlineStr"/>
       <c r="D25" t="n">
-        <v>0.2812552711997166</v>
+        <v>-0.1056961970719053</v>
       </c>
       <c r="E25" t="n">
-        <v>0.1612223986061659</v>
+        <v>0.6994142198784308</v>
       </c>
       <c r="F25" t="n">
-        <v>0.4468252236087771</v>
+        <v>-1.04977679448127</v>
       </c>
       <c r="G25" t="n">
-        <v>0.7490333789629011</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="1" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="B26" s="1" t="inlineStr"/>
-      <c r="C26" t="inlineStr"/>
-      <c r="D26" t="n">
-        <v>-0.105696197071906</v>
-      </c>
-      <c r="E26" t="n">
-        <v>0.6994142198784495</v>
-      </c>
-      <c r="F26" t="n">
-        <v>-0.6522593218995449</v>
-      </c>
-      <c r="G26" t="n">
-        <v>1.306229856967348</v>
+        <v>1.061710156781484</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A2:A19"/>
-    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A2:A18"/>
+    <mergeCell ref="A20:A22"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1639,7 +1596,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1235404575673441</v>
+        <v>0.1235404575672317</v>
       </c>
       <c r="E2" t="n">
         <v>0.1377966870439366</v>
@@ -1658,10 +1615,10 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0.01060024238988774</v>
+        <v>0.0106002423898781</v>
       </c>
       <c r="E3" t="n">
-        <v>0.01182348122121566</v>
+        <v>0.01182348122121565</v>
       </c>
     </row>
     <row r="4">
@@ -1671,16 +1628,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.2604907241031163</v>
+        <v>0.2604907241031162</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0.3329849492222581</v>
+        <v>0.3329849492228651</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>2.720383094721994e-17</v>
       </c>
     </row>
     <row r="5">
@@ -1690,16 +1647,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.7395092758968838</v>
+        <v>0.7395092758968839</v>
       </c>
       <c r="C5" t="n">
         <v>1</v>
       </c>
       <c r="D5" t="n">
-        <v>0.5328743508205099</v>
+        <v>0.532874350820025</v>
       </c>
       <c r="E5" t="n">
-        <v>0.8503798317348477</v>
+        <v>0.8503798317348475</v>
       </c>
     </row>
   </sheetData>
@@ -1756,7 +1713,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1641377906351399</v>
+        <v>0.1641377906350205</v>
       </c>
       <c r="E2" t="n">
         <v>0.1680530358447928</v>
@@ -1775,10 +1732,10 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0.006158367922456487</v>
+        <v>0.00615836792245201</v>
       </c>
       <c r="E3" t="n">
-        <v>0.006305208958143326</v>
+        <v>0.006305208958143325</v>
       </c>
     </row>
     <row r="4">
@@ -1788,16 +1745,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.2101761441374756</v>
+        <v>0.2101761441374755</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0.2660722785586033</v>
+        <v>0.266072278559137</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>1.995323420951496e-17</v>
       </c>
     </row>
     <row r="5">
@@ -1813,10 +1770,10 @@
         <v>1</v>
       </c>
       <c r="D5" t="n">
-        <v>0.5636315628838002</v>
+        <v>0.5636315628833904</v>
       </c>
       <c r="E5" t="n">
-        <v>0.8256417551970638</v>
+        <v>0.825641755197064</v>
       </c>
     </row>
   </sheetData>
@@ -1873,10 +1830,10 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1529281120668742</v>
+        <v>0.4752027330087252</v>
       </c>
       <c r="E2" t="n">
-        <v>0.09112720677979763</v>
+        <v>0.2767901661473114</v>
       </c>
     </row>
     <row r="3">
@@ -1892,10 +1849,10 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0.01013122095349617</v>
+        <v>0.0101312209534961</v>
       </c>
       <c r="E3" t="n">
-        <v>0.006036964080089547</v>
+        <v>0.005901053975171445</v>
       </c>
     </row>
     <row r="4">
@@ -1905,16 +1862,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1.125244785898144</v>
+        <v>1.125244785898142</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>1.365739122952361</v>
+        <v>1.365739122956093</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>-7.984603034434674e-17</v>
       </c>
     </row>
     <row r="5">
@@ -1924,16 +1881,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.1252447858981437</v>
+        <v>-0.1252447858981425</v>
       </c>
       <c r="C5" t="n">
         <v>1</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.5287984559727309</v>
+        <v>-0.8510730769183142</v>
       </c>
       <c r="E5" t="n">
-        <v>0.9028358291401128</v>
+        <v>0.7173087798775172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
better plot for main manuscript
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/oilcane/results/life_cycle.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/oilcane/results/life_cycle.xlsx
@@ -899,7 +899,7 @@
         <v>295214880.9294902</v>
       </c>
       <c r="D22" t="n">
-        <v>-0</v>
+        <v>3.492459654808044e-08</v>
       </c>
       <c r="E22" t="n">
         <v>394423741.1527265</v>
@@ -1460,7 +1460,7 @@
         <v>0.9496131419087513</v>
       </c>
       <c r="E22" t="n">
-        <v>-0</v>
+        <v>7.593693406881739e-17</v>
       </c>
       <c r="F22" t="n">
         <v>1.684604151485945</v>
@@ -1481,7 +1481,7 @@
         <v>0.9496131419087513</v>
       </c>
       <c r="E23" t="n">
-        <v>0</v>
+        <v>7.593693406881739e-17</v>
       </c>
       <c r="F23" t="n">
         <v>2.283251125830643</v>
@@ -1529,7 +1529,7 @@
         <v>-0.1056961970719053</v>
       </c>
       <c r="E25" t="n">
-        <v>0.6994142198784308</v>
+        <v>0.6994142198784307</v>
       </c>
       <c r="F25" t="n">
         <v>-1.04977679448127</v>
@@ -1631,13 +1631,13 @@
         <v>0.2604907241031162</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>2.816793302774396e-17</v>
       </c>
       <c r="D4" t="n">
         <v>0.3329849492228651</v>
       </c>
       <c r="E4" t="n">
-        <v>2.720383094721994e-17</v>
+        <v>2.720383094721995e-17</v>
       </c>
     </row>
     <row r="5">
@@ -1647,16 +1647,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.7395092758968839</v>
+        <v>0.7395092758968836</v>
       </c>
       <c r="C5" t="n">
         <v>1</v>
       </c>
       <c r="D5" t="n">
-        <v>0.532874350820025</v>
+        <v>0.5328743508200251</v>
       </c>
       <c r="E5" t="n">
-        <v>0.8503798317348475</v>
+        <v>0.8503798317348478</v>
       </c>
     </row>
   </sheetData>
@@ -1735,7 +1735,7 @@
         <v>0.00615836792245201</v>
       </c>
       <c r="E3" t="n">
-        <v>0.006305208958143325</v>
+        <v>0.006305208958143324</v>
       </c>
     </row>
     <row r="4">
@@ -1748,7 +1748,7 @@
         <v>0.2101761441374755</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>2.127940672645292e-17</v>
       </c>
       <c r="D4" t="n">
         <v>0.266072278559137</v>
@@ -1773,7 +1773,7 @@
         <v>0.5636315628833904</v>
       </c>
       <c r="E5" t="n">
-        <v>0.825641755197064</v>
+        <v>0.8256417551970638</v>
       </c>
     </row>
   </sheetData>
@@ -1849,7 +1849,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0101312209534961</v>
+        <v>0.01013122095349604</v>
       </c>
       <c r="E3" t="n">
         <v>0.005901053975171445</v>
@@ -1862,10 +1862,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1.125244785898142</v>
+        <v>1.125244785898143</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>1.085721907141328e-16</v>
       </c>
       <c r="D4" t="n">
         <v>1.365739122956093</v>
@@ -1881,13 +1881,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.1252447858981425</v>
+        <v>-0.1252447858981426</v>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.8510730769183142</v>
+        <v>-0.8510730769183144</v>
       </c>
       <c r="E5" t="n">
         <v>0.7173087798775172</v>

</xml_diff>